<commit_message>
fix : modify column format of sample excel file.
</commit_message>
<xml_diff>
--- a/public/assets/sms.xlsx
+++ b/public/assets/sms.xlsx
@@ -1,17 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neox/Develop/intelliJ/node/SmsSender/public/assets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="60" windowWidth="19395" windowHeight="9510"/>
+    <workbookView xWindow="600" yWindow="460" windowWidth="26360" windowHeight="15760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -328,7 +338,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,12 +368,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -376,7 +391,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -418,12 +433,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -453,12 +468,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -664,417 +679,418 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -1092,7 +1108,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1104,7 +1120,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>